<commit_message>
Add Question No.1 and No.2
</commit_message>
<xml_diff>
--- a/documents/requirement_analysis/QA票.xlsx
+++ b/documents/requirement_analysis/QA票.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273debb854664e28/デスクトップ/Projects/10031s0001/documents/requirement_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="62" documentId="11_33AE251567599405B074A2B5762D1EF2D10E3BB2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3F8C2766-8E34-4971-BEE8-FDD7665C5E27}"/>
+  <xr:revisionPtr revIDLastSave="88" documentId="11_33AE251567599405B074A2B5762D1EF2D10E3BB2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5CEF5D1-6679-4319-BDE2-CD1E3B434B1D}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="改版履歴" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -145,6 +145,42 @@
     <t>舩橋</t>
     <rPh sb="0" eb="2">
       <t>フナバシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Open</t>
+  </si>
+  <si>
+    <t>-</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>5.2.2 スタック領域について、明示的なスタック領域の確保は必要でしょうか？また、スタック領域の容量指定はありますか？</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>COMETⅡの各種レジスタ(PR, FR, GR1~4)について、領域を明示的にメモリ上に取得する想定でしょうか？</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>PHR舩橋</t>
+    <rPh sb="3" eb="5">
+      <t>フナバシ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>2.0</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>質問No.1,2を記載</t>
+    <rPh sb="0" eb="2">
+      <t>シツモン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>キサイ</t>
     </rPh>
     <phoneticPr fontId="1"/>
   </si>
@@ -246,7 +282,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -315,6 +351,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -331,10 +373,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -636,8 +674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
@@ -678,10 +716,18 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="21"/>
-      <c r="B3" s="14"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="18"/>
+      <c r="A3" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="14">
+        <v>45468</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="18" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A4" s="20"/>
@@ -856,9 +902,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -868,7 +914,10 @@
     <col min="3" max="3" width="57.875" customWidth="1"/>
     <col min="4" max="4" width="65.875" customWidth="1"/>
     <col min="5" max="5" width="72.125" customWidth="1"/>
-    <col min="6" max="9" width="7.375" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="10.625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="7" customWidth="1"/>
+    <col min="9" max="9" width="10.625" style="7" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" s="7" customFormat="1" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -891,39 +940,59 @@
         <v>6</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>3</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>4</v>
       </c>
       <c r="I1" s="6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="4"/>
+      <c r="B2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E2" s="12"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="3"/>
+      <c r="F2" s="14">
+        <v>45468</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="14"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="13"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="4"/>
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="E3" s="10"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="3"/>
+      <c r="F3" s="14">
+        <v>45468</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="14"/>
       <c r="I3" s="3"/>
     </row>
     <row r="4" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -935,8 +1004,8 @@
       <c r="D4" s="4"/>
       <c r="E4" s="9"/>
       <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="3"/>
+      <c r="G4" s="3"/>
+      <c r="H4" s="14"/>
       <c r="I4" s="3"/>
     </row>
     <row r="5" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -948,8 +1017,8 @@
       <c r="D5" s="4"/>
       <c r="E5" s="9"/>
       <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="3"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="14"/>
       <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -961,8 +1030,8 @@
       <c r="D6" s="4"/>
       <c r="E6" s="9"/>
       <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="3"/>
+      <c r="G6" s="3"/>
+      <c r="H6" s="14"/>
       <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -974,8 +1043,8 @@
       <c r="D7" s="4"/>
       <c r="E7" s="9"/>
       <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
-      <c r="H7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="14"/>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -987,8 +1056,8 @@
       <c r="D8" s="4"/>
       <c r="E8" s="9"/>
       <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="14"/>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1000,8 +1069,8 @@
       <c r="D9" s="4"/>
       <c r="E9" s="9"/>
       <c r="F9" s="14"/>
-      <c r="G9" s="14"/>
-      <c r="H9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="14"/>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1013,8 +1082,8 @@
       <c r="D10" s="4"/>
       <c r="E10" s="9"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="14"/>
-      <c r="H10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="14"/>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1026,8 +1095,8 @@
       <c r="D11" s="4"/>
       <c r="E11" s="9"/>
       <c r="F11" s="14"/>
-      <c r="G11" s="14"/>
-      <c r="H11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="14"/>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1039,8 +1108,8 @@
       <c r="D12" s="4"/>
       <c r="E12" s="9"/>
       <c r="F12" s="14"/>
-      <c r="G12" s="14"/>
-      <c r="H12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="14"/>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1052,8 +1121,8 @@
       <c r="D13" s="4"/>
       <c r="E13" s="12"/>
       <c r="F13" s="14"/>
-      <c r="G13" s="14"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="14"/>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1065,8 +1134,8 @@
       <c r="D14" s="4"/>
       <c r="E14" s="12"/>
       <c r="F14" s="14"/>
-      <c r="G14" s="14"/>
-      <c r="H14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="14"/>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1078,8 +1147,8 @@
       <c r="D15" s="4"/>
       <c r="E15" s="12"/>
       <c r="F15" s="14"/>
-      <c r="G15" s="14"/>
-      <c r="H15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="14"/>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1091,8 +1160,8 @@
       <c r="D16" s="4"/>
       <c r="E16" s="9"/>
       <c r="F16" s="14"/>
-      <c r="G16" s="14"/>
-      <c r="H16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="14"/>
       <c r="I16" s="3"/>
     </row>
     <row r="17" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1104,8 +1173,8 @@
       <c r="D17" s="4"/>
       <c r="E17" s="9"/>
       <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="14"/>
       <c r="I17" s="3"/>
     </row>
     <row r="18" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1117,8 +1186,8 @@
       <c r="D18" s="4"/>
       <c r="E18" s="9"/>
       <c r="F18" s="14"/>
-      <c r="G18" s="14"/>
-      <c r="H18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="14"/>
       <c r="I18" s="3"/>
     </row>
     <row r="19" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1130,8 +1199,8 @@
       <c r="D19" s="4"/>
       <c r="E19" s="9"/>
       <c r="F19" s="14"/>
-      <c r="G19" s="14"/>
-      <c r="H19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="14"/>
       <c r="I19" s="3"/>
     </row>
     <row r="20" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1143,8 +1212,8 @@
       <c r="D20" s="4"/>
       <c r="E20" s="9"/>
       <c r="F20" s="14"/>
-      <c r="G20" s="14"/>
-      <c r="H20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="14"/>
       <c r="I20" s="3"/>
     </row>
     <row r="21" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1156,8 +1225,8 @@
       <c r="D21" s="5"/>
       <c r="E21" s="9"/>
       <c r="F21" s="14"/>
-      <c r="G21" s="14"/>
-      <c r="H21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="14"/>
       <c r="I21" s="3"/>
     </row>
     <row r="22" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1169,8 +1238,8 @@
       <c r="D22" s="4"/>
       <c r="E22" s="9"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="3"/>
+      <c r="G22" s="3"/>
+      <c r="H22" s="14"/>
       <c r="I22" s="3"/>
     </row>
     <row r="23" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1182,8 +1251,8 @@
       <c r="D23" s="4"/>
       <c r="E23" s="9"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="14"/>
       <c r="I23" s="3"/>
     </row>
     <row r="24" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1195,8 +1264,8 @@
       <c r="D24" s="4"/>
       <c r="E24" s="9"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="14"/>
       <c r="I24" s="3"/>
     </row>
     <row r="25" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1208,8 +1277,8 @@
       <c r="D25" s="4"/>
       <c r="E25" s="9"/>
       <c r="F25" s="14"/>
-      <c r="G25" s="14"/>
-      <c r="H25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="14"/>
       <c r="I25" s="3"/>
     </row>
     <row r="26" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1221,8 +1290,8 @@
       <c r="D26" s="4"/>
       <c r="E26" s="9"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="14"/>
       <c r="I26" s="3"/>
     </row>
     <row r="27" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1234,8 +1303,8 @@
       <c r="D27" s="4"/>
       <c r="E27" s="9"/>
       <c r="F27" s="14"/>
-      <c r="G27" s="14"/>
-      <c r="H27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="14"/>
       <c r="I27" s="3"/>
     </row>
     <row r="28" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1247,8 +1316,8 @@
       <c r="D28" s="4"/>
       <c r="E28" s="9"/>
       <c r="F28" s="14"/>
-      <c r="G28" s="14"/>
-      <c r="H28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="14"/>
       <c r="I28" s="3"/>
     </row>
     <row r="29" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1260,8 +1329,8 @@
       <c r="D29" s="4"/>
       <c r="E29" s="9"/>
       <c r="F29" s="14"/>
-      <c r="G29" s="14"/>
-      <c r="H29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="14"/>
       <c r="I29" s="3"/>
     </row>
     <row r="30" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1273,8 +1342,8 @@
       <c r="D30" s="4"/>
       <c r="E30" s="9"/>
       <c r="F30" s="14"/>
-      <c r="G30" s="14"/>
-      <c r="H30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="14"/>
       <c r="I30" s="3"/>
     </row>
     <row r="31" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1286,8 +1355,8 @@
       <c r="D31" s="4"/>
       <c r="E31" s="9"/>
       <c r="F31" s="14"/>
-      <c r="G31" s="14"/>
-      <c r="H31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="14"/>
       <c r="I31" s="3"/>
     </row>
     <row r="32" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1299,8 +1368,8 @@
       <c r="D32" s="4"/>
       <c r="E32" s="9"/>
       <c r="F32" s="14"/>
-      <c r="G32" s="14"/>
-      <c r="H32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="14"/>
       <c r="I32" s="3"/>
     </row>
     <row r="33" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1312,8 +1381,8 @@
       <c r="D33" s="4"/>
       <c r="E33" s="9"/>
       <c r="F33" s="14"/>
-      <c r="G33" s="14"/>
-      <c r="H33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="14"/>
       <c r="I33" s="3"/>
     </row>
     <row r="34" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1325,8 +1394,8 @@
       <c r="D34" s="4"/>
       <c r="E34" s="9"/>
       <c r="F34" s="14"/>
-      <c r="G34" s="14"/>
-      <c r="H34" s="3"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="14"/>
       <c r="I34" s="3"/>
     </row>
     <row r="35" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1338,8 +1407,8 @@
       <c r="D35" s="4"/>
       <c r="E35" s="9"/>
       <c r="F35" s="14"/>
-      <c r="G35" s="14"/>
-      <c r="H35" s="3"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="14"/>
       <c r="I35" s="3"/>
     </row>
     <row r="36" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1351,8 +1420,8 @@
       <c r="D36" s="4"/>
       <c r="E36" s="9"/>
       <c r="F36" s="14"/>
-      <c r="G36" s="14"/>
-      <c r="H36" s="3"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="14"/>
       <c r="I36" s="3"/>
     </row>
     <row r="37" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1364,8 +1433,8 @@
       <c r="D37" s="4"/>
       <c r="E37" s="9"/>
       <c r="F37" s="14"/>
-      <c r="G37" s="14"/>
-      <c r="H37" s="3"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="14"/>
       <c r="I37" s="3"/>
     </row>
     <row r="38" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1377,8 +1446,8 @@
       <c r="D38" s="4"/>
       <c r="E38" s="9"/>
       <c r="F38" s="14"/>
-      <c r="G38" s="14"/>
-      <c r="H38" s="3"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="14"/>
       <c r="I38" s="3"/>
     </row>
     <row r="39" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1390,8 +1459,8 @@
       <c r="D39" s="4"/>
       <c r="E39" s="9"/>
       <c r="F39" s="14"/>
-      <c r="G39" s="14"/>
-      <c r="H39" s="3"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="14"/>
       <c r="I39" s="3"/>
     </row>
     <row r="40" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1403,8 +1472,8 @@
       <c r="D40" s="4"/>
       <c r="E40" s="9"/>
       <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="14"/>
       <c r="I40" s="3"/>
     </row>
     <row r="41" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1416,8 +1485,8 @@
       <c r="D41" s="4"/>
       <c r="E41" s="9"/>
       <c r="F41" s="14"/>
-      <c r="G41" s="14"/>
-      <c r="H41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="14"/>
       <c r="I41" s="3"/>
     </row>
     <row r="42" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1429,8 +1498,8 @@
       <c r="D42" s="4"/>
       <c r="E42" s="9"/>
       <c r="F42" s="14"/>
-      <c r="G42" s="14"/>
-      <c r="H42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="14"/>
       <c r="I42" s="3"/>
     </row>
     <row r="43" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1442,8 +1511,8 @@
       <c r="D43" s="4"/>
       <c r="E43" s="9"/>
       <c r="F43" s="14"/>
-      <c r="G43" s="14"/>
-      <c r="H43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="14"/>
       <c r="I43" s="3"/>
     </row>
     <row r="44" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1455,8 +1524,8 @@
       <c r="D44" s="4"/>
       <c r="E44" s="9"/>
       <c r="F44" s="14"/>
-      <c r="G44" s="14"/>
-      <c r="H44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="14"/>
       <c r="I44" s="3"/>
     </row>
     <row r="45" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1468,8 +1537,8 @@
       <c r="D45" s="4"/>
       <c r="E45" s="9"/>
       <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="14"/>
       <c r="I45" s="3"/>
     </row>
     <row r="46" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1481,8 +1550,8 @@
       <c r="D46" s="4"/>
       <c r="E46" s="9"/>
       <c r="F46" s="14"/>
-      <c r="G46" s="14"/>
-      <c r="H46" s="3"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="14"/>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1494,8 +1563,8 @@
       <c r="D47" s="4"/>
       <c r="E47" s="9"/>
       <c r="F47" s="14"/>
-      <c r="G47" s="14"/>
-      <c r="H47" s="3"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="14"/>
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1507,8 +1576,8 @@
       <c r="D48" s="4"/>
       <c r="E48" s="9"/>
       <c r="F48" s="14"/>
-      <c r="G48" s="14"/>
-      <c r="H48" s="3"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="14"/>
       <c r="I48" s="3"/>
     </row>
     <row r="49" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1520,8 +1589,8 @@
       <c r="D49" s="4"/>
       <c r="E49" s="9"/>
       <c r="F49" s="14"/>
-      <c r="G49" s="14"/>
-      <c r="H49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="14"/>
       <c r="I49" s="3"/>
     </row>
     <row r="50" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1533,8 +1602,8 @@
       <c r="D50" s="4"/>
       <c r="E50" s="9"/>
       <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="14"/>
       <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1546,8 +1615,8 @@
       <c r="D51" s="4"/>
       <c r="E51" s="9"/>
       <c r="F51" s="14"/>
-      <c r="G51" s="14"/>
-      <c r="H51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="14"/>
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1559,8 +1628,8 @@
       <c r="D52" s="4"/>
       <c r="E52" s="10"/>
       <c r="F52" s="14"/>
-      <c r="G52" s="14"/>
-      <c r="H52" s="3"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="14"/>
       <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1572,8 +1641,8 @@
       <c r="D53" s="4"/>
       <c r="E53" s="9"/>
       <c r="F53" s="14"/>
-      <c r="G53" s="14"/>
-      <c r="H53" s="3"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="14"/>
       <c r="I53" s="3"/>
     </row>
     <row r="54" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1585,8 +1654,8 @@
       <c r="D54" s="4"/>
       <c r="E54" s="9"/>
       <c r="F54" s="14"/>
-      <c r="G54" s="14"/>
-      <c r="H54" s="3"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="14"/>
       <c r="I54" s="3"/>
     </row>
     <row r="55" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1598,8 +1667,8 @@
       <c r="D55" s="4"/>
       <c r="E55" s="9"/>
       <c r="F55" s="14"/>
-      <c r="G55" s="14"/>
-      <c r="H55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="14"/>
       <c r="I55" s="3"/>
     </row>
     <row r="56" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1611,8 +1680,8 @@
       <c r="D56" s="4"/>
       <c r="E56" s="9"/>
       <c r="F56" s="14"/>
-      <c r="G56" s="14"/>
-      <c r="H56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="14"/>
       <c r="I56" s="3"/>
     </row>
     <row r="57" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1624,8 +1693,8 @@
       <c r="D57" s="4"/>
       <c r="E57" s="9"/>
       <c r="F57" s="14"/>
-      <c r="G57" s="14"/>
-      <c r="H57" s="3"/>
+      <c r="G57" s="3"/>
+      <c r="H57" s="14"/>
       <c r="I57" s="3"/>
     </row>
     <row r="58" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1637,8 +1706,8 @@
       <c r="D58" s="4"/>
       <c r="E58" s="9"/>
       <c r="F58" s="14"/>
-      <c r="G58" s="14"/>
-      <c r="H58" s="3"/>
+      <c r="G58" s="3"/>
+      <c r="H58" s="14"/>
       <c r="I58" s="3"/>
     </row>
     <row r="59" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1650,8 +1719,8 @@
       <c r="D59" s="4"/>
       <c r="E59" s="9"/>
       <c r="F59" s="14"/>
-      <c r="G59" s="14"/>
-      <c r="H59" s="3"/>
+      <c r="G59" s="3"/>
+      <c r="H59" s="14"/>
       <c r="I59" s="3"/>
     </row>
     <row r="60" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1663,8 +1732,8 @@
       <c r="D60" s="4"/>
       <c r="E60" s="9"/>
       <c r="F60" s="14"/>
-      <c r="G60" s="14"/>
-      <c r="H60" s="3"/>
+      <c r="G60" s="3"/>
+      <c r="H60" s="14"/>
       <c r="I60" s="3"/>
     </row>
     <row r="61" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1674,8 +1743,8 @@
       <c r="D61" s="2"/>
       <c r="E61" s="8"/>
       <c r="F61" s="15"/>
-      <c r="G61" s="15"/>
-      <c r="H61" s="1"/>
+      <c r="G61" s="1"/>
+      <c r="H61" s="15"/>
       <c r="I61" s="1"/>
     </row>
     <row r="62" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1685,8 +1754,8 @@
       <c r="D62" s="2"/>
       <c r="E62" s="8"/>
       <c r="F62" s="15"/>
-      <c r="G62" s="15"/>
-      <c r="H62" s="1"/>
+      <c r="G62" s="1"/>
+      <c r="H62" s="15"/>
       <c r="I62" s="1"/>
     </row>
     <row r="63" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1696,8 +1765,8 @@
       <c r="D63" s="2"/>
       <c r="E63" s="8"/>
       <c r="F63" s="15"/>
-      <c r="G63" s="15"/>
-      <c r="H63" s="1"/>
+      <c r="G63" s="1"/>
+      <c r="H63" s="15"/>
       <c r="I63" s="1"/>
     </row>
     <row r="64" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1707,8 +1776,8 @@
       <c r="D64" s="2"/>
       <c r="E64" s="8"/>
       <c r="F64" s="15"/>
-      <c r="G64" s="15"/>
-      <c r="H64" s="1"/>
+      <c r="G64" s="1"/>
+      <c r="H64" s="15"/>
       <c r="I64" s="1"/>
     </row>
     <row r="65" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1718,8 +1787,8 @@
       <c r="D65" s="2"/>
       <c r="E65" s="8"/>
       <c r="F65" s="15"/>
-      <c r="G65" s="15"/>
-      <c r="H65" s="1"/>
+      <c r="G65" s="1"/>
+      <c r="H65" s="15"/>
       <c r="I65" s="1"/>
     </row>
     <row r="66" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1729,8 +1798,8 @@
       <c r="D66" s="2"/>
       <c r="E66" s="8"/>
       <c r="F66" s="15"/>
-      <c r="G66" s="15"/>
-      <c r="H66" s="1"/>
+      <c r="G66" s="1"/>
+      <c r="H66" s="15"/>
       <c r="I66" s="1"/>
     </row>
     <row r="67" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1740,8 +1809,8 @@
       <c r="D67" s="2"/>
       <c r="E67" s="8"/>
       <c r="F67" s="15"/>
-      <c r="G67" s="15"/>
-      <c r="H67" s="1"/>
+      <c r="G67" s="1"/>
+      <c r="H67" s="15"/>
       <c r="I67" s="1"/>
     </row>
     <row r="68" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1751,8 +1820,8 @@
       <c r="D68" s="2"/>
       <c r="E68" s="8"/>
       <c r="F68" s="15"/>
-      <c r="G68" s="15"/>
-      <c r="H68" s="1"/>
+      <c r="G68" s="1"/>
+      <c r="H68" s="15"/>
       <c r="I68" s="1"/>
     </row>
     <row r="69" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
@@ -1762,8 +1831,8 @@
       <c r="D69" s="2"/>
       <c r="E69" s="8"/>
       <c r="F69" s="15"/>
-      <c r="G69" s="15"/>
-      <c r="H69" s="1"/>
+      <c r="G69" s="1"/>
+      <c r="H69" s="15"/>
       <c r="I69" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Answer No.1 and No.2
</commit_message>
<xml_diff>
--- a/documents/requirement_analysis/QA票.xlsx
+++ b/documents/requirement_analysis/QA票.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/273debb854664e28/デスクトップ/Projects/10031s0001/documents/requirement_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="88" documentId="11_33AE251567599405B074A2B5762D1EF2D10E3BB2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5CEF5D1-6679-4319-BDE2-CD1E3B434B1D}"/>
+  <xr:revisionPtr revIDLastSave="116" documentId="11_33AE251567599405B074A2B5762D1EF2D10E3BB2" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2423DCBB-08AF-4F85-B29C-B9860D280A44}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="28">
   <si>
     <t>No</t>
     <phoneticPr fontId="1"/>
@@ -149,9 +149,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Open</t>
-  </si>
-  <si>
     <t>-</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -178,6 +175,40 @@
     <t>質問No.1,2を記載</t>
     <rPh sb="0" eb="2">
       <t>シツモン</t>
+    </rPh>
+    <rPh sb="9" eb="11">
+      <t>キサイ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>37.プログラミングで展開しているcm_tbad.cで仮想メモリ領域確保しています。
+スタックは0x7FFFを先頭として、戻るようにしてください。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>はい。COMETを実装するC言語上で明に確保するようにしてください。
+cm_tbad.cで確保される領域外でよいです。</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>セック光内</t>
+    <rPh sb="3" eb="5">
+      <t>ミツウチ</t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>2.1</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>回答No.1,2を記載</t>
+    <rPh sb="0" eb="2">
+      <t>カイトウ</t>
     </rPh>
     <rPh sb="9" eb="11">
       <t>キサイ</t>
@@ -220,7 +251,7 @@
       <charset val="128"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,6 +267,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="1" tint="0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -282,7 +325,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -352,11 +395,41 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,6 +446,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -675,7 +752,7 @@
   <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.4"/>
@@ -717,7 +794,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A3" s="21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" s="14">
         <v>45468</v>
@@ -726,14 +803,22 @@
         <v>15</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="20"/>
-      <c r="B4" s="14"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="18"/>
+      <c r="A4" s="20" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="14">
+        <v>45468</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" s="18" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
       <c r="A5" s="20"/>
@@ -902,9 +987,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I69"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H10" sqref="H10"/>
+      <selection pane="bottomLeft" activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.95" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -949,51 +1034,63 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="3">
+    <row r="2" spans="1:9" s="29" customFormat="1" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="30">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="30" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="E2" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="34">
+        <v>45468</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" s="34">
+        <v>45468</v>
+      </c>
+      <c r="I2" s="30" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="23">
+        <v>2</v>
+      </c>
+      <c r="B3" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="14">
+      <c r="D3" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="25">
         <v>45468</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="14"/>
-      <c r="I2" s="3"/>
-    </row>
-    <row r="3" spans="1:9" ht="36.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="24" t="s">
+      <c r="G3" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="14">
+      <c r="H3" s="25">
         <v>45468</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="3"/>
+      <c r="I3" s="23" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="15.95" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="3">

</xml_diff>